<commit_message>
changes for send email
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testDataForOilfield.xlsx
+++ b/src/test/resources/testData/testDataForOilfield.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="6180" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="basicDetails" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
   <si>
     <t>Username</t>
   </si>
@@ -387,6 +387,12 @@
   </si>
   <si>
     <t>pankaj.yadav</t>
+  </si>
+  <si>
+    <t>Release Version</t>
+  </si>
+  <si>
+    <t>S105</t>
   </si>
 </sst>
 </file>
@@ -829,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,6 +869,14 @@
       </c>
       <c r="B3" s="6" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1021,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>